<commit_message>
Updating excel docs and commenting out code that prevents compiling
</commit_message>
<xml_diff>
--- a/Project_ESP32_MPU6050_DMP6/Data/FeatureExtract1Drop.xlsx
+++ b/Project_ESP32_MPU6050_DMP6/Data/FeatureExtract1Drop.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MIoT_Device\Project\Project_ESP32_MPU6050_DMP6_DataGather\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MIoT_Project\Project_ESP32_MPU6050_DMP6\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D21C24-9F16-4824-A886-752D7293A74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742EEE69-207F-4BA7-A917-90227B0055AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{18F599CE-0939-4435-A581-4464DE41BE50}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{18F599CE-0939-4435-A581-4464DE41BE50}"/>
   </bookViews>
   <sheets>
     <sheet name="FeatureExtract1" sheetId="2" r:id="rId1"/>
@@ -20011,7 +20011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A51BF6-52C1-437E-9405-35CD554A83D0}">
   <dimension ref="A1:AL151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M64" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD52"/>
     </sheetView>
   </sheetViews>

</xml_diff>